<commit_message>
Aggiornamento casi test 08/04/2025
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#WEBCENTRYRISXX/GE_Medical_System_Italia_SPA/WEBCENTRYRIS/1.25/report-checklist.xlsx
+++ b/GATEWAY/A1#111#WEBCENTRYRISXX/GE_Medical_System_Italia_SPA/WEBCENTRYRIS/1.25/report-checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11730" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -692,12 +692,6 @@
     <t>subject_application_vendor: GE_MEDICAL_SYSTEM_ITALIA_SPA</t>
   </si>
   <si>
-    <t>2025-02-23T13:18:35</t>
-  </si>
-  <si>
-    <t>9c60ca9b602b6b34</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -728,70 +722,74 @@
     <t>Il codice fiscale viene automaticamente convertito in maiuscolo</t>
   </si>
   <si>
-    <t>2025-02-27T10:01:41</t>
-  </si>
-  <si>
-    <t>6d3f39b4199e1a59</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180101.4.4.022dd5df074a956beb6cbbc83af5ffbf2ff20215775ea822470582692c4a4f78.5beabf0c9d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Eccezione  durante la validazione del documento clinico FSE:
 "{title}": Errore vocabolario.
 "{detail}": È stata trovata almeno una versione non gestita di un dizionario: [2.16.840.1.113883.2.9.6.2.7 vISCO-08]
 Continuare comunque con la generazione del referto?</t>
   </si>
   <si>
-    <t>2025-02-27T18:26:23</t>
-  </si>
-  <si>
-    <t>f79f8018f0cf6b6f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eccezione  durante la validazione del documento clinico FSE:
-"{title}": Errore semantico.
-"{detail}": [ERRORE-b7| Sezione Dicom Object Catalog: La sezione deve avere l'elemento 'entry' di tipo 'act'.],[W005 | Sezione Esame Eseguito: l'entry/act/code può essere valorizzato secondo i sistemi di codifica
-   LOINC @codeSystem='2.16.840.1.113883.6.1'
-   ICD-9-CM @codeSystem='2.16.840.1.113883.6.103']
-Continuare comunque con la generazione del referto?
-</t>
-  </si>
-  <si>
-    <t>2025-02-28T10:21:17</t>
-  </si>
-  <si>
-    <t>121cebbccab5e487</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180101.4.4.53b4fa66cebaa9f9c962c0132baaa7dfcea8c3f46484e029fc572f253f9f208d.3723285114^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Eccezione  durante la validazione del documento clinico FSE:
 "{title}": Errore vocabolario.
 "{detail}": Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 123.A]
 Continuare comunque con la generazione del referto?</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.180101.4.4.9f61799a4536ff9bb33098a275bd94d12679e0b6a5484cdc8e7582b53212fce1.7f9c1702ee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-03-11T16:37:33</t>
-  </si>
-  <si>
-    <t>114c97199199e2e4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180101.4.4.357960146e181f072c606b1431caf2cae985cfea8d38dce518b8950e80250ead.b99af1c325^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-03-11T18:09:07</t>
-  </si>
-  <si>
-    <t>e1e2199b69f67452</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.180101.4.4.0fdd104e3c79f7cda3b6abc890702b4feccb8c8a7e06603058a81b1a3d8e4710.3a50bd5781^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-04-08T12:57:09</t>
+  </si>
+  <si>
+    <t>0a6a70036042d394</t>
+  </si>
+  <si>
+    <t>3086ec9083801c3d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180101.4.4.670e0e2292494cadea5a168257a01e73be38a92669967ab14409298b0321d566.c332999a73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-04-08T16:42:10</t>
+  </si>
+  <si>
+    <t>52a7efbb6ca148e9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180101.4.4.041c4cb44f4c9bddbb450cb8b54dcb788e0c6dbe80fafdaf3b70dcc72290e617.fee1a722d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eccezione  durante la validazione del documento clinico FSE:
+"{title}": Errore semantico.
+"{detail}":[ERRORE-b7| Sezione Dicom Object Catalog: La sezione deve avere l'elemento 'entry' di tipo 'act'.]
+Continuare comunque con la generazione del referto?
+</t>
+  </si>
+  <si>
+    <t>2025-04-08T16:51:12</t>
+  </si>
+  <si>
+    <t>1a73f68c02c8df9e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180101.4.4.8273370c48107f6985f1d1c99c71a0709a047011613197530a63a002f9501641.61b7c1783b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-04-08T16:58:14</t>
+  </si>
+  <si>
+    <t>9931fe049d4f2daf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180101.4.4.951d2d320d2e41deb7c3530969885c8aca1ba9d3003e875ef79b5415eeb0fb10.05dd2e9b9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-04-08T17:02:36</t>
+  </si>
+  <si>
+    <t>5c46ce011f6527da</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180101.4.4.3808f711ac84baf34bcf371ccfa56ea0c52f803b42391bb337159e83e3ea1f72.a97bdcfc3d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-04-08T16:06:21</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2801,11 +2799,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W608"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2813,7 +2811,7 @@
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
@@ -3109,16 +3107,16 @@
         <v>44</v>
       </c>
       <c r="F10" s="33">
-        <v>45711</v>
+        <v>45755</v>
       </c>
       <c r="G10" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="I10" s="37" t="s">
         <v>145</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="I10" s="37" t="s">
-        <v>147</v>
       </c>
       <c r="J10" s="29" t="s">
         <v>51</v>
@@ -3132,7 +3130,7 @@
         <v>51</v>
       </c>
       <c r="O10" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="P10" s="29" t="s">
         <v>51</v>
@@ -3144,7 +3142,7 @@
         <v>93</v>
       </c>
       <c r="S10" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T10" s="29"/>
       <c r="U10" s="34"/>
@@ -3226,7 +3224,7 @@
         <v>51</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P12" s="29" t="s">
         <v>93</v>
@@ -3238,7 +3236,7 @@
         <v>93</v>
       </c>
       <c r="S12" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T12" s="29"/>
       <c r="U12" s="34" t="s">
@@ -3317,7 +3315,7 @@
         <v>104</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M14" s="29"/>
       <c r="N14" s="29"/>
@@ -3514,16 +3512,16 @@
         <v>122</v>
       </c>
       <c r="F19" s="33">
-        <v>45715</v>
+        <v>45755</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I19" s="37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>51</v>
@@ -3537,7 +3535,7 @@
         <v>51</v>
       </c>
       <c r="O19" s="29" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="P19" s="29" t="s">
         <v>51</v>
@@ -3549,7 +3547,7 @@
         <v>93</v>
       </c>
       <c r="S19" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T19" s="29"/>
       <c r="U19" s="34"/>
@@ -3780,7 +3778,7 @@
         <v>126</v>
       </c>
       <c r="F25" s="33">
-        <v>45715</v>
+        <v>45755</v>
       </c>
       <c r="G25" s="33" t="s">
         <v>157</v>
@@ -3789,7 +3787,7 @@
         <v>158</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J25" s="29" t="s">
         <v>51</v>
@@ -3803,7 +3801,7 @@
         <v>51</v>
       </c>
       <c r="O25" s="29" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P25" s="29" t="s">
         <v>51</v>
@@ -3815,7 +3813,7 @@
         <v>93</v>
       </c>
       <c r="S25" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T25" s="29"/>
       <c r="U25" s="34"/>
@@ -4005,16 +4003,16 @@
         <v>132</v>
       </c>
       <c r="F30" s="33">
-        <v>45716</v>
+        <v>45755</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J30" s="29" t="s">
         <v>51</v>
@@ -4028,7 +4026,7 @@
         <v>51</v>
       </c>
       <c r="O30" s="29" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="P30" s="29" t="s">
         <v>51</v>
@@ -4040,7 +4038,7 @@
         <v>93</v>
       </c>
       <c r="S30" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T30" s="29"/>
       <c r="U30" s="34"/>
@@ -4107,16 +4105,16 @@
         <v>116</v>
       </c>
       <c r="F32" s="33">
-        <v>45727</v>
+        <v>45755</v>
       </c>
       <c r="G32" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="H32" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="I32" s="37" t="s">
         <v>166</v>
-      </c>
-      <c r="I32" s="37" t="s">
-        <v>167</v>
       </c>
       <c r="J32" s="29" t="s">
         <v>51</v>
@@ -4154,16 +4152,16 @@
         <v>117</v>
       </c>
       <c r="F33" s="33">
-        <v>45727</v>
+        <v>45755</v>
       </c>
       <c r="G33" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="H33" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="H33" s="33" t="s">
+      <c r="I33" s="37" t="s">
         <v>169</v>
-      </c>
-      <c r="I33" s="37" t="s">
-        <v>170</v>
       </c>
       <c r="J33" s="29" t="s">
         <v>51</v>
@@ -8607,7 +8605,7 @@
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10785,12 +10783,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10966,19 +10965,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11002,17 +11008,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>